<commit_message>
pushing all working statistical tests
</commit_message>
<xml_diff>
--- a/mnt/data/DATAS.xlsx
+++ b/mnt/data/DATAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehdi_aks/Desktop/Mémoire R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alirachidi/Documents/elyprojet/mnt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E23E56-9A3F-394F-BBCA-04288A271722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA92553-5115-184A-A6B7-BE116F83F29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AA26FB2D-B090-4049-A72C-D0176A6BBE36}"/>
+    <workbookView xWindow="2580" yWindow="600" windowWidth="20360" windowHeight="14300" xr2:uid="{AA26FB2D-B090-4049-A72C-D0176A6BBE36}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="262">
   <si>
     <t>Mehdi</t>
   </si>
@@ -820,6 +820,9 @@
   <si>
     <t>Ecart_TpsReacMoy_Droite</t>
   </si>
+  <si>
+    <t>Pas2_CorrelOeilDirecteur_Lateralite</t>
+  </si>
 </sst>
 </file>
 
@@ -1507,7 +1510,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1825,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E518B0-A901-924D-8966-5CF13261B1BE}">
   <dimension ref="A1:FL285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="75" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="AT31" sqref="AT31"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="75" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1965,7 +1968,7 @@
         <v>115</v>
       </c>
       <c r="AK1" s="99" t="s">
-        <v>124</v>
+        <v>261</v>
       </c>
       <c r="AL1" s="100" t="s">
         <v>116</v>

</xml_diff>